<commit_message>
chore: Actualizacion de signos y sintomas
</commit_message>
<xml_diff>
--- a/files/BD_SIGNOS_SINTOMAS.xlsx
+++ b/files/BD_SIGNOS_SINTOMAS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopez\Desktop\UPC\Tesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c8778beaa6210769/Escritorio/Github/UPC-Works/api-modelocombinado-aliviate/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7835942A-A2C3-40E2-8F64-35CB6F9359CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{7835942A-A2C3-40E2-8F64-35CB6F9359CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EED95F55-CFBB-4E01-B304-3B100233AD58}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E13CB23-8FEA-4C5D-A460-EBE554DD7E97}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1E13CB23-8FEA-4C5D-A460-EBE554DD7E97}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>SIGNOS_SINTOMAS</t>
   </si>
@@ -144,12 +144,6 @@
   </si>
   <si>
     <t>Terapia de reemplazo hormonal con levotiroxina para restablecer los niveles normales de hormonas tiroideas</t>
-  </si>
-  <si>
-    <t>Dolor abdominal, diarrea crónica, sangrado rectal, pérdida de peso, fatiga, fiebre, llagas en la boca</t>
-  </si>
-  <si>
-    <t>colitis ulcerosa o enfermedad de Crohn</t>
   </si>
   <si>
     <t>Fatiga extrema, debilidad muscular, pérdida de peso, náuseas, mareos, cambios en la piel y el cabello, baja presión arterial</t>
@@ -395,6 +389,86 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -428,86 +502,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -522,19 +516,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3ECE28DE-BBD7-44D5-9F5B-060E0FCF5849}" name="Tabla2" displayName="Tabla2" ref="A1:C21" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
-  <autoFilter ref="A1:C21" xr:uid="{3ECE28DE-BBD7-44D5-9F5B-060E0FCF5849}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3ECE28DE-BBD7-44D5-9F5B-060E0FCF5849}" name="Tabla2" displayName="Tabla2" ref="A1:C20" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C20" xr:uid="{3ECE28DE-BBD7-44D5-9F5B-060E0FCF5849}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{92C4E337-F2FB-46A1-ACE7-EA5CD18CBF59}" name="SIGNOS_SINTOMAS" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{70670F05-CBB8-4D9C-BA58-3F18A1111E8C}" name="ENFERMEDAD" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{F04E878F-0B10-4F61-8869-1936FFA49AA5}" name="TRATAMIENTO" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{92C4E337-F2FB-46A1-ACE7-EA5CD18CBF59}" name="SIGNOS_SINTOMAS" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{70670F05-CBB8-4D9C-BA58-3F18A1111E8C}" name="ENFERMEDAD" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{F04E878F-0B10-4F61-8869-1936FFA49AA5}" name="TRATAMIENTO" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -830,15 +824,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{626DC38D-1BAE-4451-8F9B-9D1DED951016}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="33.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -849,7 +846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -860,7 +857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -871,7 +868,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -882,7 +879,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -893,7 +890,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -904,7 +901,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -915,7 +912,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -926,7 +923,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -937,7 +934,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -948,7 +945,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -959,7 +956,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -970,7 +967,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -978,43 +975,43 @@
         <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>47</v>
       </c>
@@ -1022,51 +1019,40 @@
         <v>48</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="2" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="B20" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="C20" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>